<commit_message>
Moved ByBit related code to ByBitExchange.py file.
</commit_message>
<xml_diff>
--- a/Output/Statistics.xlsx
+++ b/Output/Statistics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,100 +441,105 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Exchange</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Symbol</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>From</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>To</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Interval</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>TP %</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>SL %</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Maker Fee %</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Taker Fee %</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Precision Crossing</t>
-        </is>
-      </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Strategy</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Total Trades</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Success Rate</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Loss Idx</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Win Idx</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Wins $</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Losses $</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Fees $</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Total P/L</t>
         </is>
@@ -546,73 +551,80 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>ByBit</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>BTCUSD</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2021-11-01</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>2021-10-01</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>2021-12-01</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>10000</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
       <c r="H2" t="n">
-        <v>0.6666666666666666</v>
+        <v>6</v>
       </c>
       <c r="I2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" t="n">
         <v>-0.025</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.075</v>
       </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>4</v>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>MACD</t>
+        </is>
       </c>
       <c r="M2" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>26.7%</t>
-        </is>
-      </c>
-      <c r="P2" t="n">
-        <v>-10</v>
+        <v>6</v>
+      </c>
+      <c r="O2" t="n">
+        <v>13</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>53.8%</t>
+        </is>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="S2" t="n">
-        <v>-733.333333333333</v>
+        <v>4200</v>
       </c>
       <c r="T2" t="n">
-        <v>185</v>
+        <v>-2400</v>
       </c>
       <c r="U2" t="n">
-        <v>-518.333333333333</v>
+        <v>132.05</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1667.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for Binance.
</commit_message>
<xml_diff>
--- a/Output/Statistics.xlsx
+++ b/Output/Statistics.xlsx
@@ -556,17 +556,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BTCUSD</t>
+          <t>BTCUSDT</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-09-01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2021-12-01</t>
+          <t>2022-01-01</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -591,40 +591,40 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>MACD</t>
+          <t>Early MACD</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="N2" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="O2" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>53.8%</t>
+          <t>42.3%</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="R2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S2" t="n">
-        <v>4200</v>
+        <v>6600</v>
       </c>
       <c r="T2" t="n">
-        <v>-2400</v>
+        <v>-6000</v>
       </c>
       <c r="U2" t="n">
-        <v>132.05</v>
+        <v>278.35</v>
       </c>
       <c r="V2" t="n">
-        <v>1667.95</v>
+        <v>321.65</v>
       </c>
     </row>
     <row r="3">
@@ -633,22 +633,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ByBit</t>
+          <t>Binance</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BTCUSD</t>
+          <t>BTCUSDT</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2021-10-01</t>
+          <t>2021-09-01</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2021-12-01</t>
+          <t>2022-01-01</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -673,40 +673,40 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>MACD Precise</t>
+          <t>Early MACD</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N3" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="O3" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>53.8%</t>
+          <t>38.5%</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="R3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S3" t="n">
-        <v>4200</v>
+        <v>6000</v>
       </c>
       <c r="T3" t="n">
-        <v>-2400</v>
+        <v>-6400</v>
       </c>
       <c r="U3" t="n">
-        <v>132.05</v>
+        <v>287.9</v>
       </c>
       <c r="V3" t="n">
-        <v>1667.95</v>
+        <v>-687.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>